<commit_message>
unique_gen program handles new merging dataset
</commit_message>
<xml_diff>
--- a/Scoring.xlsx
+++ b/Scoring.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC333F-8A47-4F25-B125-34AC5A687778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D74BE3D-44FA-45D6-A841-D6E7C2CD8092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="3" r:id="rId1"/>
-    <sheet name="scoring" sheetId="2" r:id="rId2"/>
+    <sheet name="b" sheetId="4" r:id="rId2"/>
+    <sheet name="scoring" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="194">
   <si>
     <t>Industry</t>
   </si>
@@ -605,6 +606,9 @@
   </si>
   <si>
     <t>40-65</t>
+  </si>
+  <si>
+    <t>Unique ID</t>
   </si>
 </sst>
 </file>
@@ -1839,10 +1843,802 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4314A7D-6514-4B52-8947-CDFD0131C954}">
+  <dimension ref="A1:AB12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" customWidth="1"/>
+    <col min="17" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="26.44140625" customWidth="1"/>
+    <col min="21" max="21" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" customWidth="1"/>
+    <col min="24" max="24" width="20.109375" customWidth="1"/>
+    <col min="25" max="25" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="10">
+        <v>44819</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="13">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="10">
+        <v>44819</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="3">
+        <v>42200</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AB3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="10">
+        <v>44820</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="3">
+        <v>71010</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AB4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="10">
+        <v>44821</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="3">
+        <v>46050</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="10">
+        <v>44822</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="3">
+        <v>50480</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="10">
+        <v>44823</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="3">
+        <v>47810</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AB7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="10">
+        <v>44757</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="3">
+        <v>96000</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="T8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AB8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="10">
+        <v>44788</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="3">
+        <v>87000</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="T9" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AB9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="10">
+        <v>44197</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="3">
+        <v>81300</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AB10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="10">
+        <v>43863</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="3">
+        <v>43300</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AB11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="10">
+        <v>44782</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" s="3">
+        <v>40150</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AB12">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1" xr:uid="{4C1B3E43-4E0A-4D1E-AF51-0B76C3CAA80C}"/>
+    <hyperlink ref="O4" r:id="rId2" xr:uid="{03FF6000-D1F9-4F73-A23B-ABEF1528B88C}"/>
+    <hyperlink ref="P3" r:id="rId3" display="B@B" xr:uid="{77F467C6-D151-464E-8CC1-7BE0690F2F1A}"/>
+    <hyperlink ref="P5" r:id="rId4" display="B@B" xr:uid="{566BDAEE-EC2E-487B-B6B9-A4A6EB0133AF}"/>
+    <hyperlink ref="P7" r:id="rId5" display="B@B" xr:uid="{2B3DC337-5247-4FC4-BD70-2F7C43936036}"/>
+    <hyperlink ref="P9" r:id="rId6" display="B@B" xr:uid="{5E1F0586-E36E-4697-B88D-639B3E030722}"/>
+    <hyperlink ref="P11" r:id="rId7" display="B@B" xr:uid="{683ABEC4-BA4A-4720-AFDC-88102CC2B6DB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFDA3F8-1A08-4412-8D92-78F99D48F60E}">
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>